<commit_message>
- 04_model-rule.js: reverted logic to how it was at 62b79. Added changes to incorporate decision service on top of it.
- model-rule.json
set cachable to false

- model-feel-decision-table-blank-object-payload.js
modified test to check for any JS_FEEL_ERR

- model-rule-base-entity-inheritance-tests.js
fixed test case execution

-populator1.xlsx
changed hit policy to F
</commit_message>
<xml_diff>
--- a/test/model-rule-data/populator1.xlsx
+++ b/test/model-rule-data/populator1.xlsx
@@ -41,9 +41,6 @@
     <t>Action</t>
   </si>
   <si>
-    <t>U</t>
-  </si>
-  <si>
     <t>gender</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>"men"</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -119,7 +119,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -404,7 +405,7 @@
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,17 +430,17 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -447,13 +448,13 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -461,13 +462,13 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -475,13 +476,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -489,13 +490,13 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
         <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -503,13 +504,13 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
         <v>9</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -517,13 +518,13 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>